<commit_message>
Troublesooting CarDriveline, before setup sheets
are fast
</commit_message>
<xml_diff>
--- a/torquecurves.xlsx
+++ b/torquecurves.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\MATLAB\Combined LapSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -738,11 +738,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="260580896"/>
-        <c:axId val="260581288"/>
+        <c:axId val="417135160"/>
+        <c:axId val="417135552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="260580896"/>
+        <c:axId val="417135160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,13 +772,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260581288"/>
+        <c:crossAx val="417135552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="260581288"/>
+        <c:axId val="417135552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -790,7 +790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260580896"/>
+        <c:crossAx val="417135160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1265,11 +1265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261930888"/>
-        <c:axId val="261933240"/>
+        <c:axId val="372104792"/>
+        <c:axId val="372108320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261930888"/>
+        <c:axId val="372104792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,13 +1299,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261933240"/>
+        <c:crossAx val="372108320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261933240"/>
+        <c:axId val="372108320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,7 +1317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261930888"/>
+        <c:crossAx val="372104792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2056,11 +2056,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261931672"/>
-        <c:axId val="261935200"/>
+        <c:axId val="372105576"/>
+        <c:axId val="372107144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261931672"/>
+        <c:axId val="372105576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,13 +2090,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261935200"/>
+        <c:crossAx val="372107144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261935200"/>
+        <c:axId val="372107144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2108,7 +2108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261931672"/>
+        <c:crossAx val="372105576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2859,11 +2859,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261935592"/>
-        <c:axId val="261936376"/>
+        <c:axId val="372100088"/>
+        <c:axId val="372103616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261935592"/>
+        <c:axId val="372100088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2893,13 +2893,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261936376"/>
+        <c:crossAx val="372103616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261936376"/>
+        <c:axId val="372103616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2911,7 +2911,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261935592"/>
+        <c:crossAx val="372100088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3746,11 +3746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261937160"/>
-        <c:axId val="336684472"/>
+        <c:axId val="372104008"/>
+        <c:axId val="372100872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261937160"/>
+        <c:axId val="372104008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3780,13 +3780,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336684472"/>
+        <c:crossAx val="372100872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336684472"/>
+        <c:axId val="372100872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3798,7 +3798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261937160"/>
+        <c:crossAx val="372104008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4273,11 +4273,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336683296"/>
-        <c:axId val="336684864"/>
+        <c:axId val="372101656"/>
+        <c:axId val="372107536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336683296"/>
+        <c:axId val="372101656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4307,13 +4307,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336684864"/>
+        <c:crossAx val="372107536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336684864"/>
+        <c:axId val="372107536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4325,7 +4325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336683296"/>
+        <c:crossAx val="372101656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5328,11 +5328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337942104"/>
-        <c:axId val="337938184"/>
+        <c:axId val="372108712"/>
+        <c:axId val="372096952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337942104"/>
+        <c:axId val="372108712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5362,13 +5362,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337938184"/>
+        <c:crossAx val="372096952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337938184"/>
+        <c:axId val="372096952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5380,7 +5380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337942104"/>
+        <c:crossAx val="372108712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6287,11 +6287,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337941712"/>
-        <c:axId val="337937400"/>
+        <c:axId val="372112240"/>
+        <c:axId val="372109104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337941712"/>
+        <c:axId val="372112240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6321,13 +6321,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337937400"/>
+        <c:crossAx val="372109104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337937400"/>
+        <c:axId val="372109104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6339,7 +6339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337941712"/>
+        <c:crossAx val="372112240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7210,11 +7210,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337940928"/>
-        <c:axId val="337941320"/>
+        <c:axId val="372109888"/>
+        <c:axId val="372110280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337940928"/>
+        <c:axId val="372109888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7244,13 +7244,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337941320"/>
+        <c:crossAx val="372110280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337941320"/>
+        <c:axId val="372110280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7262,7 +7262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337940928"/>
+        <c:crossAx val="372109888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7941,11 +7941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337939752"/>
-        <c:axId val="337937792"/>
+        <c:axId val="372111456"/>
+        <c:axId val="372111848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337939752"/>
+        <c:axId val="372111456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7975,13 +7975,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337937792"/>
+        <c:crossAx val="372111848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337937792"/>
+        <c:axId val="372111848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7993,7 +7993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337939752"/>
+        <c:crossAx val="372111456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9068,11 +9068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337940144"/>
-        <c:axId val="337935048"/>
+        <c:axId val="429063168"/>
+        <c:axId val="429063560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337940144"/>
+        <c:axId val="429063168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9102,13 +9102,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337935048"/>
+        <c:crossAx val="429063560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337935048"/>
+        <c:axId val="429063560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9120,7 +9120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337940144"/>
+        <c:crossAx val="429063168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9727,11 +9727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336682904"/>
-        <c:axId val="336683688"/>
+        <c:axId val="417132808"/>
+        <c:axId val="417123008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336682904"/>
+        <c:axId val="417132808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9761,13 +9761,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336683688"/>
+        <c:crossAx val="417123008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336683688"/>
+        <c:axId val="417123008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9779,7 +9779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336682904"/>
+        <c:crossAx val="417132808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10421,11 +10421,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337937008"/>
-        <c:axId val="337940536"/>
+        <c:axId val="429068656"/>
+        <c:axId val="429063952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337937008"/>
+        <c:axId val="429068656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10455,13 +10455,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337940536"/>
+        <c:crossAx val="429063952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337940536"/>
+        <c:axId val="429063952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10473,7 +10473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337937008"/>
+        <c:crossAx val="429068656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11416,11 +11416,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337935832"/>
-        <c:axId val="337936224"/>
+        <c:axId val="429069048"/>
+        <c:axId val="429069440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337935832"/>
+        <c:axId val="429069048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11450,13 +11450,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337936224"/>
+        <c:crossAx val="429069440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337936224"/>
+        <c:axId val="429069440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11468,7 +11468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="337935832"/>
+        <c:crossAx val="429069048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12471,11 +12471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338700200"/>
-        <c:axId val="338698632"/>
+        <c:axId val="429072968"/>
+        <c:axId val="429071792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338700200"/>
+        <c:axId val="429072968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12505,13 +12505,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338698632"/>
+        <c:crossAx val="429071792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338698632"/>
+        <c:axId val="429071792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12523,7 +12523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338700200"/>
+        <c:crossAx val="429072968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14018,11 +14018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338692360"/>
-        <c:axId val="338690792"/>
+        <c:axId val="429066304"/>
+        <c:axId val="429066696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338692360"/>
+        <c:axId val="429066304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14052,13 +14052,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338690792"/>
+        <c:crossAx val="429066696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338690792"/>
+        <c:axId val="429066696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14070,7 +14070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338692360"/>
+        <c:crossAx val="429066304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14171,7 +14171,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>600</c:v>
@@ -14558,7 +14558,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>2.0053999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.3754</c:v>
@@ -14956,7 +14956,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>600</c:v>
@@ -15343,7 +15343,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
                 <c:pt idx="0">
-                  <c:v>0.1909177456207159</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.27137090632140137</c:v>
@@ -15733,11 +15733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="338696672"/>
-        <c:axId val="338701768"/>
+        <c:axId val="429065912"/>
+        <c:axId val="429068264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338696672"/>
+        <c:axId val="429065912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15768,13 +15768,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338701768"/>
+        <c:crossAx val="429068264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338701768"/>
+        <c:axId val="429068264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15786,7 +15786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338696672"/>
+        <c:crossAx val="429065912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16381,11 +16381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336682120"/>
-        <c:axId val="336684080"/>
+        <c:axId val="417128104"/>
+        <c:axId val="298693840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336682120"/>
+        <c:axId val="417128104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16415,13 +16415,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336684080"/>
+        <c:crossAx val="298693840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336684080"/>
+        <c:axId val="298693840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16433,7 +16433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336682120"/>
+        <c:crossAx val="417128104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17460,11 +17460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336686432"/>
-        <c:axId val="336680160"/>
+        <c:axId val="298696192"/>
+        <c:axId val="298697760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336686432"/>
+        <c:axId val="298696192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17494,13 +17494,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336680160"/>
+        <c:crossAx val="298697760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336680160"/>
+        <c:axId val="298697760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17512,7 +17512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336686432"/>
+        <c:crossAx val="298696192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18923,11 +18923,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336680552"/>
-        <c:axId val="336680944"/>
+        <c:axId val="372106360"/>
+        <c:axId val="372097344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336680552"/>
+        <c:axId val="372106360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18957,13 +18957,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336680944"/>
+        <c:crossAx val="372097344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336680944"/>
+        <c:axId val="372097344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18975,7 +18975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336680552"/>
+        <c:crossAx val="372106360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19654,11 +19654,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="336682512"/>
-        <c:axId val="336685648"/>
+        <c:axId val="372098128"/>
+        <c:axId val="372102048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="336682512"/>
+        <c:axId val="372098128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19688,13 +19688,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336685648"/>
+        <c:crossAx val="372102048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336685648"/>
+        <c:axId val="372102048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19706,7 +19706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="336682512"/>
+        <c:crossAx val="372098128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20937,11 +20937,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261932456"/>
-        <c:axId val="261932848"/>
+        <c:axId val="372100480"/>
+        <c:axId val="372098520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261932456"/>
+        <c:axId val="372100480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20971,13 +20971,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261932848"/>
+        <c:crossAx val="372098520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261932848"/>
+        <c:axId val="372098520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20989,7 +20989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261932456"/>
+        <c:crossAx val="372100480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21896,11 +21896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261935984"/>
-        <c:axId val="261933632"/>
+        <c:axId val="372101264"/>
+        <c:axId val="372099304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261935984"/>
+        <c:axId val="372101264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21930,13 +21930,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261933632"/>
+        <c:crossAx val="372099304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261933632"/>
+        <c:axId val="372099304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21948,7 +21948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261935984"/>
+        <c:crossAx val="372101264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22627,11 +22627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261937944"/>
-        <c:axId val="261938336"/>
+        <c:axId val="372106752"/>
+        <c:axId val="372099696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261937944"/>
+        <c:axId val="372106752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22661,13 +22661,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261938336"/>
+        <c:crossAx val="372099696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261938336"/>
+        <c:axId val="372099696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22679,7 +22679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261937944"/>
+        <c:crossAx val="372106752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -38350,7 +38350,7 @@
   <dimension ref="A1:X147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I123" sqref="I123"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38388,14 +38388,14 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C4">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2.0053999999999998</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>(C4*E4)/5252</f>
-        <v>0.1909177456207159</v>
+        <f>0.001</f>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finding values for Michael Delay, realized it was combustion fuel
</commit_message>
<xml_diff>
--- a/torquecurves.xlsx
+++ b/torquecurves.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340" firstSheet="20" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340" firstSheet="20" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Rennteam Uni Stuttgart" sheetId="1" r:id="rId1"/>
@@ -770,11 +770,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353383424"/>
-        <c:axId val="353392832"/>
+        <c:axId val="38328944"/>
+        <c:axId val="269216416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353383424"/>
+        <c:axId val="38328944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,13 +804,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353392832"/>
+        <c:crossAx val="269216416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353392832"/>
+        <c:axId val="269216416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353383424"/>
+        <c:crossAx val="38328944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1297,11 +1297,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353396360"/>
-        <c:axId val="353396752"/>
+        <c:axId val="345843928"/>
+        <c:axId val="345843144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353396360"/>
+        <c:axId val="345843928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1331,13 +1331,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353396752"/>
+        <c:crossAx val="345843144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353396752"/>
+        <c:axId val="345843144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353396360"/>
+        <c:crossAx val="345843928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2088,11 +2088,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353395576"/>
-        <c:axId val="353394792"/>
+        <c:axId val="345843536"/>
+        <c:axId val="345844712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353395576"/>
+        <c:axId val="345843536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2122,13 +2122,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353394792"/>
+        <c:crossAx val="345844712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353394792"/>
+        <c:axId val="345844712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,7 +2140,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353395576"/>
+        <c:crossAx val="345843536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2891,11 +2891,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="397093344"/>
-        <c:axId val="397097264"/>
+        <c:axId val="267839048"/>
+        <c:axId val="267839832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="397093344"/>
+        <c:axId val="267839048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2925,13 +2925,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397097264"/>
+        <c:crossAx val="267839832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="397097264"/>
+        <c:axId val="267839832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2943,7 +2943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397093344"/>
+        <c:crossAx val="267839048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3778,11 +3778,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="397101968"/>
-        <c:axId val="397096480"/>
+        <c:axId val="346128088"/>
+        <c:axId val="346130048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="397101968"/>
+        <c:axId val="346128088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3812,13 +3812,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397096480"/>
+        <c:crossAx val="346130048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="397096480"/>
+        <c:axId val="346130048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3830,7 +3830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397101968"/>
+        <c:crossAx val="346128088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4305,11 +4305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="397098832"/>
-        <c:axId val="397103928"/>
+        <c:axId val="346130440"/>
+        <c:axId val="346128480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="397098832"/>
+        <c:axId val="346130440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4339,13 +4339,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397103928"/>
+        <c:crossAx val="346128480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="397103928"/>
+        <c:axId val="346128480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,7 +4357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="397098832"/>
+        <c:crossAx val="346130440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5360,11 +5360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354967040"/>
-        <c:axId val="354970568"/>
+        <c:axId val="346130832"/>
+        <c:axId val="346127304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354967040"/>
+        <c:axId val="346130832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5394,13 +5394,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354970568"/>
+        <c:crossAx val="346127304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354970568"/>
+        <c:axId val="346127304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5412,7 +5412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354967040"/>
+        <c:crossAx val="346130832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6319,11 +6319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354968608"/>
-        <c:axId val="354970960"/>
+        <c:axId val="346000008"/>
+        <c:axId val="345993736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354968608"/>
+        <c:axId val="346000008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6353,13 +6353,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354970960"/>
+        <c:crossAx val="345993736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354970960"/>
+        <c:axId val="345993736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6371,7 +6371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354968608"/>
+        <c:crossAx val="346000008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7242,11 +7242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354963512"/>
-        <c:axId val="136084512"/>
+        <c:axId val="345994912"/>
+        <c:axId val="345994128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354963512"/>
+        <c:axId val="345994912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7276,13 +7276,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136084512"/>
+        <c:crossAx val="345994128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136084512"/>
+        <c:axId val="345994128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7294,7 +7294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="354963512"/>
+        <c:crossAx val="345994912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7973,11 +7973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136088040"/>
-        <c:axId val="136082160"/>
+        <c:axId val="345995696"/>
+        <c:axId val="346000400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136088040"/>
+        <c:axId val="345995696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8007,13 +8007,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136082160"/>
+        <c:crossAx val="346000400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136082160"/>
+        <c:axId val="346000400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8025,7 +8025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136088040"/>
+        <c:crossAx val="345995696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9100,11 +9100,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136083336"/>
-        <c:axId val="136084120"/>
+        <c:axId val="345996872"/>
+        <c:axId val="345996088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136083336"/>
+        <c:axId val="345996872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9134,13 +9134,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136084120"/>
+        <c:crossAx val="345996088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136084120"/>
+        <c:axId val="345996088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9152,7 +9152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136083336"/>
+        <c:crossAx val="345996872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9759,11 +9759,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353385384"/>
-        <c:axId val="353384208"/>
+        <c:axId val="267836696"/>
+        <c:axId val="267841008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353385384"/>
+        <c:axId val="267836696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9793,13 +9793,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353384208"/>
+        <c:crossAx val="267841008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353384208"/>
+        <c:axId val="267841008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9811,7 +9811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353385384"/>
+        <c:crossAx val="267836696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10453,11 +10453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137510856"/>
-        <c:axId val="137509288"/>
+        <c:axId val="345994520"/>
+        <c:axId val="345996480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137510856"/>
+        <c:axId val="345994520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10487,13 +10487,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137509288"/>
+        <c:crossAx val="345996480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137509288"/>
+        <c:axId val="345996480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10505,7 +10505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137510856"/>
+        <c:crossAx val="345994520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11448,11 +11448,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137511640"/>
-        <c:axId val="271431928"/>
+        <c:axId val="345997656"/>
+        <c:axId val="345998048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137511640"/>
+        <c:axId val="345997656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11482,13 +11482,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="271431928"/>
+        <c:crossAx val="345998048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="271431928"/>
+        <c:axId val="345998048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11500,7 +11500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137511640"/>
+        <c:crossAx val="345997656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12503,11 +12503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="270273328"/>
-        <c:axId val="270275680"/>
+        <c:axId val="345998832"/>
+        <c:axId val="345999224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="270273328"/>
+        <c:axId val="345998832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12538,13 +12538,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="270275680"/>
+        <c:crossAx val="345999224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="270275680"/>
+        <c:axId val="345999224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12556,7 +12556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="270273328"/>
+        <c:crossAx val="345998832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14051,11 +14051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391720496"/>
-        <c:axId val="391718536"/>
+        <c:axId val="347578360"/>
+        <c:axId val="347579144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="391720496"/>
+        <c:axId val="347578360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14085,13 +14085,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391718536"/>
+        <c:crossAx val="347579144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="391718536"/>
+        <c:axId val="347579144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14103,7 +14103,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391720496"/>
+        <c:crossAx val="347578360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15766,11 +15766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391718928"/>
-        <c:axId val="391728336"/>
+        <c:axId val="347586592"/>
+        <c:axId val="347581496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="391718928"/>
+        <c:axId val="347586592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15800,13 +15800,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391728336"/>
+        <c:crossAx val="347581496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="391728336"/>
+        <c:axId val="347581496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15818,7 +15818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391718928"/>
+        <c:crossAx val="347586592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15914,101 +15914,119 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>CalPolySLO!$C$4:$C$34</c:f>
+              <c:f>CalPolySLO!$C$4:$C$40</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0" formatCode="0.00">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
                   <c:v>3500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8" formatCode="0.00">
                   <c:v>4008.5714285714284</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>4261.2857142857147</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>4509.5183673469392</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>4760.9047619047615</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>5013.6190476190477</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13" formatCode="0.00">
                   <c:v>5263.4285714285716</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14" formatCode="0.00">
                   <c:v>5513.2380952380954</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>5763.0476190476193</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>6015.7619047619046</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17" formatCode="0.00">
                   <c:v>6265.8204081632648</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18" formatCode="0.00">
                   <c:v>6517.1238095238095</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19" formatCode="0.00">
                   <c:v>6771</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20" formatCode="0.00">
                   <c:v>7018.1537414965987</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21" formatCode="0.00">
                   <c:v>7267.7972789115638</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22" formatCode="0.00">
                   <c:v>7519.8476190476194</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23" formatCode="0.00">
                   <c:v>7770.6530612244896</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24" formatCode="0.00">
                   <c:v>8020.0476190476193</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25" formatCode="0.00">
                   <c:v>8269.4421768707489</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26" formatCode="0.00">
                   <c:v>8520.2476190476191</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27" formatCode="0.00">
                   <c:v>8771.4680272108853</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28" formatCode="0.00">
                   <c:v>9022.1904761904771</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29" formatCode="0.00">
                   <c:v>9269.178231292517</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30" formatCode="0.00">
                   <c:v>9525.2952380952374</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31" formatCode="0.00">
                   <c:v>9772.2829931972792</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32" formatCode="0.00">
                   <c:v>10024.333333333334</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33" formatCode="0.00">
                   <c:v>10273.810884353741</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34" formatCode="0.00">
                   <c:v>10527.189115646259</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35" formatCode="0.00">
                   <c:v>10775.504761904762</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="36" formatCode="0.00">
                   <c:v>11002.574149659864</c:v>
                 </c:pt>
               </c:numCache>
@@ -16016,101 +16034,119 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CalPolySLO!$E$4:$E$34</c:f>
+              <c:f>CalPolySLO!$E$4:$E$40</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>24.736699999999999</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.736699999999999</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.736721311475414</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>24.83704918032787</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>25.227540983606552</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>25.186229508196721</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>25.176393442622963</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13" formatCode="0.00">
                   <c:v>27.871475409836062</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.282295081967206</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>27.282295081967199</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>25.49409836065573</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>24.541967213114759</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17" formatCode="0.00">
                   <c:v>27.582295081967214</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18" formatCode="0.00">
                   <c:v>31.602295081967203</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19" formatCode="0.00">
                   <c:v>31.9327868852459</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20" formatCode="0.00">
                   <c:v>31.591475409836065</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21" formatCode="0.00">
                   <c:v>30.680655737704917</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22" formatCode="0.00">
                   <c:v>29.734426229508188</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23" formatCode="0.00">
                   <c:v>29.317377049180323</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24" formatCode="0.00">
                   <c:v>29.369508196721316</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25" formatCode="0.00">
                   <c:v>29.134426229508204</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26" formatCode="0.00">
                   <c:v>29.247540983606562</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27" formatCode="0.00">
                   <c:v>28.88065573770491</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28" formatCode="0.00">
                   <c:v>28.750819672131154</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29" formatCode="0.00">
                   <c:v>28.513770491803275</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30" formatCode="0.00">
                   <c:v>28.340089418777936</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31" formatCode="0.00">
                   <c:v>27.780245901639336</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32" formatCode="0.00">
                   <c:v>27.3172131147541</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33" formatCode="0.00">
                   <c:v>26.282274590163933</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34" formatCode="0.00">
                   <c:v>25.862042875157634</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35" formatCode="0.00">
                   <c:v>24.214880201765446</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="36" formatCode="0.00">
                   <c:v>23.163416738567733</c:v>
                 </c:pt>
               </c:numCache>
@@ -16129,101 +16165,119 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>CalPolySLO!$C$4:$C$34</c:f>
+              <c:f>CalPolySLO!$C$4:$C$40</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0" formatCode="0.00">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00">
                   <c:v>3500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8" formatCode="0.00">
                   <c:v>4008.5714285714284</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>4261.2857142857147</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>4509.5183673469392</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>4760.9047619047615</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>5013.6190476190477</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13" formatCode="0.00">
                   <c:v>5263.4285714285716</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14" formatCode="0.00">
                   <c:v>5513.2380952380954</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>5763.0476190476193</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>6015.7619047619046</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17" formatCode="0.00">
                   <c:v>6265.8204081632648</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18" formatCode="0.00">
                   <c:v>6517.1238095238095</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19" formatCode="0.00">
                   <c:v>6771</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20" formatCode="0.00">
                   <c:v>7018.1537414965987</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21" formatCode="0.00">
                   <c:v>7267.7972789115638</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22" formatCode="0.00">
                   <c:v>7519.8476190476194</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23" formatCode="0.00">
                   <c:v>7770.6530612244896</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24" formatCode="0.00">
                   <c:v>8020.0476190476193</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25" formatCode="0.00">
                   <c:v>8269.4421768707489</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26" formatCode="0.00">
                   <c:v>8520.2476190476191</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27" formatCode="0.00">
                   <c:v>8771.4680272108853</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28" formatCode="0.00">
                   <c:v>9022.1904761904771</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29" formatCode="0.00">
                   <c:v>9269.178231292517</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30" formatCode="0.00">
                   <c:v>9525.2952380952374</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31" formatCode="0.00">
                   <c:v>9772.2829931972792</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32" formatCode="0.00">
                   <c:v>10024.333333333334</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33" formatCode="0.00">
                   <c:v>10273.810884353741</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34" formatCode="0.00">
                   <c:v>10527.189115646259</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35" formatCode="0.00">
                   <c:v>10775.504761904762</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="36" formatCode="0.00">
                   <c:v>11002.574149659864</c:v>
                 </c:pt>
               </c:numCache>
@@ -16231,101 +16285,119 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CalPolySLO!$F$4:$F$34</c:f>
+              <c:f>CalPolySLO!$F$4:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>3.6565901207703</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.4820856816451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3075812425198601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1330768033946299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.958572364269401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.7840679251442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.609563486018899</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>18.880219780219782</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>20.15189696442172</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>21.661092808181913</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="11">
                   <c:v>22.83115765422696</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
                   <c:v>24.033672070503762</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
                   <c:v>27.932124904798169</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
                   <c:v>28.639335219236202</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>27.974810140354691</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="16">
                   <c:v>28.110935153954959</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="17">
                   <c:v>32.90664650201284</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
                   <c:v>39.214788597541059</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>41.168488194973342</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>42.215124018838303</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>42.456356870851927</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>42.573944075726246</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>43.376840387335434</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
                   <c:v>44.848601349145909</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="25">
                   <c:v>45.873087026128047</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>47.44788488738984</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="27">
                   <c:v>48.234148592567252</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="28">
                   <c:v>49.389827004678502</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29">
                   <c:v>50.323537839812225</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="30">
                   <c:v>51.39903251863646</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>51.690103688390806</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>52.139537319116535</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>51.412627332444778</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34">
                   <c:v>51.838274231480639</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35">
                   <c:v>49.681560724119741</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="36">
                   <c:v>48.525744521242189</c:v>
                 </c:pt>
               </c:numCache>
@@ -16341,11 +16413,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391727552"/>
-        <c:axId val="391720888"/>
+        <c:axId val="347577184"/>
+        <c:axId val="347587376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="391727552"/>
+        <c:axId val="347577184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16369,19 +16441,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391720888"/>
+        <c:crossAx val="347587376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="391720888"/>
+        <c:axId val="347587376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16393,7 +16466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391727552"/>
+        <c:crossAx val="347577184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16988,11 +17061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353387736"/>
-        <c:axId val="353389304"/>
+        <c:axId val="267834344"/>
+        <c:axId val="267835128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353387736"/>
+        <c:axId val="267834344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17022,13 +17095,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353389304"/>
+        <c:crossAx val="267835128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353389304"/>
+        <c:axId val="267835128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17040,7 +17113,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353387736"/>
+        <c:crossAx val="267834344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18067,11 +18140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353385776"/>
-        <c:axId val="353382248"/>
+        <c:axId val="267837480"/>
+        <c:axId val="267837872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353385776"/>
+        <c:axId val="267837480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18095,20 +18168,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353382248"/>
+        <c:crossAx val="267837872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353382248"/>
+        <c:axId val="267837872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18120,7 +18192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353385776"/>
+        <c:crossAx val="267837480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19531,11 +19603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353388912"/>
-        <c:axId val="353381856"/>
+        <c:axId val="345848240"/>
+        <c:axId val="345845104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353388912"/>
+        <c:axId val="345848240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19565,13 +19637,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353381856"/>
+        <c:crossAx val="345845104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353381856"/>
+        <c:axId val="345845104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19583,7 +19655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353388912"/>
+        <c:crossAx val="345848240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20262,11 +20334,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353384600"/>
-        <c:axId val="353392440"/>
+        <c:axId val="345841968"/>
+        <c:axId val="345847456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353384600"/>
+        <c:axId val="345841968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20296,13 +20368,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353392440"/>
+        <c:crossAx val="345847456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353392440"/>
+        <c:axId val="345847456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20314,7 +20386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353384600"/>
+        <c:crossAx val="345841968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21545,11 +21617,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353384992"/>
-        <c:axId val="353389696"/>
+        <c:axId val="345845888"/>
+        <c:axId val="345845496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353384992"/>
+        <c:axId val="345845888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21579,13 +21651,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353389696"/>
+        <c:crossAx val="345845496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353389696"/>
+        <c:axId val="345845496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21597,7 +21669,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353384992"/>
+        <c:crossAx val="345845888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22504,11 +22576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353387344"/>
-        <c:axId val="353391656"/>
+        <c:axId val="345846280"/>
+        <c:axId val="345841576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353387344"/>
+        <c:axId val="345846280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22538,13 +22610,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353391656"/>
+        <c:crossAx val="345841576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353391656"/>
+        <c:axId val="345841576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22556,7 +22628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353387344"/>
+        <c:crossAx val="345846280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23235,11 +23307,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353395968"/>
-        <c:axId val="353397144"/>
+        <c:axId val="345844320"/>
+        <c:axId val="345842360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353395968"/>
+        <c:axId val="345844320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23269,13 +23341,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353397144"/>
+        <c:crossAx val="345842360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353397144"/>
+        <c:axId val="345842360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23287,7 +23359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="353395968"/>
+        <c:crossAx val="345844320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -35981,7 +36053,7 @@
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -41739,10 +41811,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41778,369 +41850,435 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5">
-        <v>24.736699999999999</v>
+        <v>2</v>
       </c>
       <c r="F4" s="5">
-        <v>0.1</v>
+        <v>3.6565901207703</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C5" s="5">
-        <v>3500</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5">
-        <v>24.736699999999999</v>
+      <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
       </c>
       <c r="F5" s="5">
-        <v>16</v>
+        <v>5.4820856816451</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="5">
-        <v>4008.5714285714284</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5">
-        <v>24.736721311475414</v>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
       </c>
       <c r="F6" s="5">
-        <v>18.880219780219782</v>
+        <v>7.3075812425198601</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="5">
-        <v>4261.2857142857147</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5">
-        <v>24.83704918032787</v>
+      <c r="C7">
+        <v>1500</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
       </c>
       <c r="F7" s="5">
-        <v>20.15189696442172</v>
+        <v>9.1330768033946299</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="5">
-        <v>4509.5183673469392</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
-        <v>25.227540983606552</v>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
       </c>
       <c r="F8" s="5">
-        <v>21.661092808181913</v>
+        <v>10.958572364269401</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="5">
-        <v>4760.9047619047615</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
-        <v>25.186229508196721</v>
+      <c r="C9">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
       </c>
       <c r="F9" s="5">
-        <v>22.83115765422696</v>
+        <v>12.7840679251442</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="5">
-        <v>5013.6190476190477</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
-        <v>25.176393442622963</v>
+      <c r="C10">
+        <v>3000</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
       </c>
       <c r="F10" s="5">
-        <v>24.033672070503762</v>
+        <v>14.609563486018899</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" s="5">
-        <v>5263.4285714285716</v>
+        <v>3500</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5">
-        <v>27.871475409836062</v>
+        <v>23</v>
       </c>
       <c r="F11" s="5">
-        <v>27.932124904798169</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C12" s="5">
-        <v>5513.2380952380954</v>
+        <v>4008.5714285714284</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5">
-        <v>27.282295081967206</v>
+        <v>24</v>
       </c>
       <c r="F12" s="5">
-        <v>28.639335219236202</v>
+        <v>18.880219780219782</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" s="5">
-        <v>5763.0476190476193</v>
+        <v>4261.2857142857147</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5">
-        <v>25.49409836065573</v>
+        <v>24.83704918032787</v>
       </c>
       <c r="F13" s="5">
-        <v>27.974810140354691</v>
+        <v>20.15189696442172</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" s="5">
-        <v>6015.7619047619046</v>
+        <v>4509.5183673469392</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5">
-        <v>24.541967213114759</v>
+        <v>25.227540983606552</v>
       </c>
       <c r="F14" s="5">
-        <v>28.110935153954959</v>
+        <v>21.661092808181913</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C15" s="5">
-        <v>6265.8204081632648</v>
+        <v>4760.9047619047615</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5">
-        <v>27.582295081967214</v>
+        <v>25.186229508196721</v>
       </c>
       <c r="F15" s="5">
-        <v>32.90664650201284</v>
+        <v>22.83115765422696</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C16" s="5">
-        <v>6517.1238095238095</v>
+        <v>5013.6190476190477</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5">
-        <v>31.602295081967203</v>
+        <v>25.176393442622963</v>
       </c>
       <c r="F16" s="5">
-        <v>39.214788597541059</v>
+        <v>24.033672070503762</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C17" s="5">
-        <v>6771</v>
+        <v>5263.4285714285716</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5">
-        <v>31.9327868852459</v>
+        <v>27.871475409836062</v>
       </c>
       <c r="F17" s="5">
-        <v>41.168488194973342</v>
+        <v>27.932124904798169</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C18" s="5">
-        <v>7018.1537414965987</v>
+        <v>5513.2380952380954</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5">
-        <v>31.591475409836065</v>
+        <v>27.282295081967199</v>
       </c>
       <c r="F18" s="5">
-        <v>42.215124018838303</v>
+        <v>28.639335219236202</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C19" s="5">
-        <v>7267.7972789115638</v>
+        <v>5763.0476190476193</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5">
-        <v>30.680655737704917</v>
+        <v>25.49409836065573</v>
       </c>
       <c r="F19" s="5">
-        <v>42.456356870851927</v>
+        <v>27.974810140354691</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C20" s="5">
-        <v>7519.8476190476194</v>
+        <v>6015.7619047619046</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5">
-        <v>29.734426229508188</v>
+        <v>24.541967213114759</v>
       </c>
       <c r="F20" s="5">
-        <v>42.573944075726246</v>
+        <v>28.110935153954959</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C21" s="5">
-        <v>7770.6530612244896</v>
+        <v>6265.8204081632648</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5">
-        <v>29.317377049180323</v>
+        <v>27.582295081967214</v>
       </c>
       <c r="F21" s="5">
-        <v>43.376840387335434</v>
+        <v>32.90664650201284</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C22" s="5">
-        <v>8020.0476190476193</v>
+        <v>6517.1238095238095</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5">
-        <v>29.369508196721316</v>
+        <v>31.602295081967203</v>
       </c>
       <c r="F22" s="5">
-        <v>44.848601349145909</v>
+        <v>39.214788597541059</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C23" s="5">
-        <v>8269.4421768707489</v>
+        <v>6771</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5">
-        <v>29.134426229508204</v>
+        <v>31.9327868852459</v>
       </c>
       <c r="F23" s="5">
-        <v>45.873087026128047</v>
+        <v>41.168488194973342</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C24" s="5">
-        <v>8520.2476190476191</v>
+        <v>7018.1537414965987</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5">
-        <v>29.247540983606562</v>
+        <v>31.591475409836065</v>
       </c>
       <c r="F24" s="5">
-        <v>47.44788488738984</v>
+        <v>42.215124018838303</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C25" s="5">
-        <v>8771.4680272108853</v>
+        <v>7267.7972789115638</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5">
-        <v>28.88065573770491</v>
+        <v>30.680655737704917</v>
       </c>
       <c r="F25" s="5">
-        <v>48.234148592567252</v>
+        <v>42.456356870851927</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C26" s="5">
-        <v>9022.1904761904771</v>
+        <v>7519.8476190476194</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5">
-        <v>28.750819672131154</v>
+        <v>29.734426229508188</v>
       </c>
       <c r="F26" s="5">
-        <v>49.389827004678502</v>
+        <v>42.573944075726246</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C27" s="5">
-        <v>9269.178231292517</v>
+        <v>7770.6530612244896</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5">
-        <v>28.513770491803275</v>
+        <v>29.317377049180323</v>
       </c>
       <c r="F27" s="5">
-        <v>50.323537839812225</v>
+        <v>43.376840387335434</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C28" s="5">
-        <v>9525.2952380952374</v>
+        <v>8020.0476190476193</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5">
-        <v>28.340089418777936</v>
+        <v>29.369508196721316</v>
       </c>
       <c r="F28" s="5">
-        <v>51.39903251863646</v>
+        <v>44.848601349145909</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C29" s="5">
-        <v>9772.2829931972792</v>
+        <v>8269.4421768707489</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5">
-        <v>27.780245901639336</v>
+        <v>29.134426229508204</v>
       </c>
       <c r="F29" s="5">
-        <v>51.690103688390806</v>
+        <v>45.873087026128047</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C30" s="5">
-        <v>10024.333333333334</v>
+        <v>8520.2476190476191</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5">
-        <v>27.3172131147541</v>
+        <v>29.247540983606562</v>
       </c>
       <c r="F30" s="5">
-        <v>52.139537319116535</v>
+        <v>47.44788488738984</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C31" s="5">
-        <v>10273.810884353741</v>
+        <v>8771.4680272108853</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5">
-        <v>26.282274590163933</v>
+        <v>28.88065573770491</v>
       </c>
       <c r="F31" s="5">
-        <v>51.412627332444778</v>
+        <v>48.234148592567252</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C32" s="5">
-        <v>10527.189115646259</v>
+        <v>9022.1904761904771</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5">
-        <v>25.862042875157634</v>
+        <v>28.750819672131154</v>
       </c>
       <c r="F32" s="5">
-        <v>51.838274231480639</v>
+        <v>49.389827004678502</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C33" s="5">
-        <v>10775.504761904762</v>
+        <v>9269.178231292517</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5">
-        <v>24.214880201765446</v>
+        <v>28.513770491803275</v>
       </c>
       <c r="F33" s="5">
-        <v>49.681560724119741</v>
+        <v>50.323537839812225</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C34" s="5">
-        <v>11002.574149659864</v>
+        <v>9525.2952380952374</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5">
+        <v>28.340089418777936</v>
+      </c>
+      <c r="F34" s="5">
+        <v>51.39903251863646</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35" s="5">
+        <v>9772.2829931972792</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5">
+        <v>27.780245901639336</v>
+      </c>
+      <c r="F35" s="5">
+        <v>51.690103688390806</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36" s="5">
+        <v>10024.333333333334</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5">
+        <v>27.3172131147541</v>
+      </c>
+      <c r="F36" s="5">
+        <v>52.139537319116535</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37" s="5">
+        <v>10273.810884353741</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5">
+        <v>26.282274590163933</v>
+      </c>
+      <c r="F37" s="5">
+        <v>51.412627332444778</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="5">
+        <v>10527.189115646259</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5">
+        <v>25.862042875157634</v>
+      </c>
+      <c r="F38" s="5">
+        <v>51.838274231480639</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39" s="5">
+        <v>10775.504761904762</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5">
+        <v>24.214880201765446</v>
+      </c>
+      <c r="F39" s="5">
+        <v>49.681560724119741</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="5">
+        <v>11002.574149659864</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5">
         <v>23.163416738567733</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F40" s="5">
         <v>48.525744521242189</v>
       </c>
     </row>

</xml_diff>